<commit_message>
refs #668 Kriterienliste überprüft
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
+++ b/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29980" windowHeight="19000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Leeres Kriterienblatt" sheetId="1" r:id="rId1"/>
     <sheet name="Beispiele" sheetId="2" r:id="rId2"/>
     <sheet name="Tips" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -377,9 +377,6 @@
     <t>Kriterien Domain Analyse Dok (SE Dok: Domain Analyse: GUI)</t>
   </si>
   <si>
-    <t>Gesammtnote</t>
-  </si>
-  <si>
     <t>Code sinnvoll dokumentiert</t>
   </si>
   <si>
@@ -490,13 +487,7 @@
     <t>2 Dokumente (Bericht und Technischer Teil) mit gleicher Seitennummerierung sind ok</t>
   </si>
   <si>
-    <t>empfehlenswert (üben für Bachelorarbeit)</t>
-  </si>
-  <si>
     <t>Management Summary</t>
-  </si>
-  <si>
-    <t>Komplexität von Project Flip 2.0 ist hoch</t>
   </si>
   <si>
     <t>Domain Model ist korrektes UML</t>
@@ -627,6 +618,15 @@
   </si>
   <si>
     <t>Screenshot in Dokumentation</t>
+  </si>
+  <si>
+    <t>Übernahme aus SA</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Gesamtnote</t>
   </si>
 </sst>
 </file>
@@ -3826,33 +3826,33 @@
   </sheetPr>
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B201" sqref="B201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="120.83203125" customWidth="1"/>
-    <col min="3" max="3" width="7.5" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
-    <col min="5" max="5" width="61.5" style="60" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="71" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="120.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" style="60" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E1" s="61"/>
       <c r="F1" s="71"/>
     </row>
-    <row r="2" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="2" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="3"/>
       <c r="E2" s="61"/>
       <c r="F2" s="71"/>
     </row>
-    <row r="3" spans="1:6" s="18" customFormat="1" ht="30">
+    <row r="3" spans="1:6" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="24" t="s">
         <v>82</v>
       </c>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="F3" s="71"/>
     </row>
-    <row r="4" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="4" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A4" s="29" t="s">
         <v>0</v>
       </c>
@@ -3886,15 +3886,15 @@
         <v>3</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" ht="30">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A5" s="31">
         <v>1</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" s="40">
         <v>5</v>
@@ -3903,12 +3903,12 @@
       <c r="E5"/>
       <c r="F5" s="72"/>
     </row>
-    <row r="6" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="6" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A6" s="31">
         <v>2</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C6" s="40">
         <v>5</v>
@@ -3917,7 +3917,7 @@
       <c r="E6"/>
       <c r="F6" s="72"/>
     </row>
-    <row r="7" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="7" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A7" s="31">
         <v>3</v>
       </c>
@@ -3931,42 +3931,44 @@
       <c r="E7"/>
       <c r="F7" s="72"/>
     </row>
-    <row r="8" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="8" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="5">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="40">
         <v>5</v>
       </c>
       <c r="D8"/>
       <c r="E8"/>
-      <c r="F8" s="73">
-        <v>40812</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="4" customFormat="1" ht="30">
+      <c r="F8" s="73" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A9" s="5">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C9" s="40">
         <v>5</v>
       </c>
       <c r="D9"/>
       <c r="E9"/>
-      <c r="F9" s="72"/>
-    </row>
-    <row r="10" spans="1:6" s="4" customFormat="1" ht="30">
+      <c r="F9" s="72" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="9">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C10" s="40">
         <v>5</v>
@@ -3975,7 +3977,7 @@
       <c r="E10"/>
       <c r="F10" s="72"/>
     </row>
-    <row r="11" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="11" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A11" s="9">
         <v>7</v>
       </c>
@@ -3989,7 +3991,7 @@
       <c r="E11"/>
       <c r="F11" s="72"/>
     </row>
-    <row r="12" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="12" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="5">
         <v>8</v>
       </c>
@@ -4003,12 +4005,12 @@
       <c r="E12"/>
       <c r="F12" s="72"/>
     </row>
-    <row r="13" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="13" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A13" s="5">
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C13" s="40">
         <v>5</v>
@@ -4017,7 +4019,7 @@
       <c r="E13"/>
       <c r="F13" s="72"/>
     </row>
-    <row r="14" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="14" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -4031,12 +4033,12 @@
       <c r="E14"/>
       <c r="F14" s="72"/>
     </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="15" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A15" s="9">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C15" s="40">
         <v>5</v>
@@ -4045,12 +4047,12 @@
       <c r="E15"/>
       <c r="F15" s="72"/>
     </row>
-    <row r="16" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="16" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="9">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C16" s="40">
         <v>5</v>
@@ -4059,7 +4061,7 @@
       <c r="E16"/>
       <c r="F16" s="72"/>
     </row>
-    <row r="17" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="17" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="5">
         <v>13</v>
       </c>
@@ -4073,7 +4075,7 @@
       <c r="E17"/>
       <c r="F17" s="72"/>
     </row>
-    <row r="18" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="18" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="5">
         <v>14</v>
       </c>
@@ -4087,7 +4089,7 @@
       <c r="E18"/>
       <c r="F18" s="72"/>
     </row>
-    <row r="19" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="19" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A19" s="25">
         <v>15</v>
       </c>
@@ -4101,7 +4103,7 @@
       <c r="E19"/>
       <c r="F19" s="72"/>
     </row>
-    <row r="20" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="20" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="30">
         <v>16</v>
       </c>
@@ -4115,7 +4117,7 @@
       <c r="E20"/>
       <c r="F20" s="72"/>
     </row>
-    <row r="21" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="21" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A21" s="25">
         <v>17</v>
       </c>
@@ -4129,12 +4131,12 @@
       <c r="E21"/>
       <c r="F21" s="72"/>
     </row>
-    <row r="22" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="22" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="25">
         <v>18</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C22" s="40">
         <v>5</v>
@@ -4143,12 +4145,12 @@
       <c r="E22"/>
       <c r="F22" s="72"/>
     </row>
-    <row r="23" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="23" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A23" s="25">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C23" s="40">
         <v>5</v>
@@ -4157,7 +4159,7 @@
       <c r="E23"/>
       <c r="F23" s="72"/>
     </row>
-    <row r="24" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="24" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A24" s="25">
         <v>20</v>
       </c>
@@ -4171,12 +4173,12 @@
       <c r="E24"/>
       <c r="F24" s="72"/>
     </row>
-    <row r="25" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="25" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A25" s="25">
         <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C25" s="40">
         <v>5</v>
@@ -4185,12 +4187,12 @@
       <c r="E25"/>
       <c r="F25" s="72"/>
     </row>
-    <row r="26" spans="1:6" ht="32" customHeight="1">
+    <row r="26" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>22</v>
       </c>
       <c r="B26" s="78" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C26" s="40">
         <v>5</v>
@@ -4198,12 +4200,12 @@
       <c r="E26"/>
       <c r="F26" s="72"/>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A27" s="25">
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C27" s="40">
         <v>5</v>
@@ -4212,12 +4214,12 @@
       <c r="E27"/>
       <c r="F27" s="72"/>
     </row>
-    <row r="28" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="28" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="25">
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C28" s="40">
         <v>5</v>
@@ -4226,12 +4228,12 @@
       <c r="E28"/>
       <c r="F28" s="72"/>
     </row>
-    <row r="29" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="25">
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C29" s="40">
         <v>5</v>
@@ -4240,7 +4242,7 @@
       <c r="E29"/>
       <c r="F29" s="72"/>
     </row>
-    <row r="30" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="30" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A30" s="25">
         <v>26</v>
       </c>
@@ -4254,7 +4256,7 @@
       <c r="E30"/>
       <c r="F30" s="72"/>
     </row>
-    <row r="31" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="31" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A31" s="25">
         <v>27</v>
       </c>
@@ -4268,12 +4270,12 @@
       <c r="E31" s="43"/>
       <c r="F31" s="72"/>
     </row>
-    <row r="32" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A32" s="21">
         <v>28</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C32" s="40">
         <v>5</v>
@@ -4282,12 +4284,12 @@
       <c r="E32" s="42"/>
       <c r="F32" s="72"/>
     </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="33" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A33" s="57">
         <v>29</v>
       </c>
       <c r="B33" s="58" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C33" s="40">
         <v>5</v>
@@ -4296,14 +4298,14 @@
       <c r="E33" s="63"/>
       <c r="F33" s="72"/>
     </row>
-    <row r="34" spans="1:6" ht="15">
+    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="15"/>
       <c r="C34" s="45"/>
       <c r="D34" s="46"/>
       <c r="E34" s="47"/>
     </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="23">
+    <row r="35" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
         <v>83</v>
       </c>
@@ -4319,7 +4321,7 @@
       </c>
       <c r="F35" s="26"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>0</v>
       </c>
@@ -4336,7 +4338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A37" s="14">
         <v>1</v>
       </c>
@@ -4348,16 +4350,16 @@
       </c>
       <c r="D37" s="33"/>
       <c r="E37" s="47" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F37" s="71"/>
     </row>
-    <row r="38" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="38" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A38" s="12">
         <v>2</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C38" s="32">
         <v>5</v>
@@ -4366,23 +4368,23 @@
       <c r="E38" s="42"/>
       <c r="F38" s="71"/>
     </row>
-    <row r="39" spans="1:6" s="4" customFormat="1" ht="30">
+    <row r="39" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A39" s="12">
         <v>3</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C39" s="32">
         <v>5</v>
       </c>
       <c r="D39" s="33"/>
       <c r="E39" s="42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F39" s="71"/>
     </row>
-    <row r="40" spans="1:6" ht="15">
+    <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>4</v>
       </c>
@@ -4395,7 +4397,7 @@
       <c r="D40" s="33"/>
       <c r="E40" s="43"/>
     </row>
-    <row r="41" spans="1:6" ht="15">
+    <row r="41" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>5</v>
       </c>
@@ -4408,12 +4410,12 @@
       <c r="D41" s="33"/>
       <c r="E41" s="43"/>
     </row>
-    <row r="42" spans="1:6" ht="15">
+    <row r="42" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9">
         <v>6</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="32">
         <v>5</v>
@@ -4421,7 +4423,7 @@
       <c r="D42" s="33"/>
       <c r="E42" s="43"/>
     </row>
-    <row r="43" spans="1:6" ht="15">
+    <row r="43" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>7</v>
       </c>
@@ -4434,12 +4436,12 @@
       <c r="D43" s="33"/>
       <c r="E43" s="43"/>
     </row>
-    <row r="44" spans="1:6" ht="15">
+    <row r="44" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C44" s="32">
         <v>5</v>
@@ -4447,12 +4449,12 @@
       <c r="D44" s="33"/>
       <c r="E44" s="43"/>
     </row>
-    <row r="45" spans="1:6" ht="15">
+    <row r="45" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9">
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C45" s="32">
         <v>5</v>
@@ -4460,7 +4462,7 @@
       <c r="D45" s="33"/>
       <c r="E45" s="43"/>
     </row>
-    <row r="46" spans="1:6" ht="15">
+    <row r="46" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="9">
         <v>11</v>
       </c>
@@ -4473,12 +4475,12 @@
       <c r="D46" s="33"/>
       <c r="E46" s="43"/>
     </row>
-    <row r="47" spans="1:6" ht="28">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="26">
         <v>13</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" s="32">
         <v>5</v>
@@ -4486,7 +4488,7 @@
       <c r="D47" s="33"/>
       <c r="E47" s="43"/>
     </row>
-    <row r="48" spans="1:6" s="7" customFormat="1" ht="15">
+    <row r="48" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="26">
         <v>14</v>
       </c>
@@ -4498,16 +4500,16 @@
       </c>
       <c r="D48" s="33"/>
       <c r="E48" s="43" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F48" s="71"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="64"/>
     </row>
-    <row r="50" spans="1:6" ht="23">
+    <row r="50" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A50" s="23" t="s">
         <v>84</v>
       </c>
@@ -4523,7 +4525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>0</v>
       </c>
@@ -4540,7 +4542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15">
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>1</v>
       </c>
@@ -4553,7 +4555,7 @@
       <c r="D52" s="33"/>
       <c r="E52" s="65"/>
     </row>
-    <row r="53" spans="1:6" s="7" customFormat="1" ht="15">
+    <row r="53" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>2</v>
       </c>
@@ -4567,7 +4569,7 @@
       <c r="E53" s="38"/>
       <c r="F53" s="71"/>
     </row>
-    <row r="54" spans="1:6" ht="15">
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
         <v>3</v>
       </c>
@@ -4580,7 +4582,7 @@
       <c r="D54" s="33"/>
       <c r="E54" s="38"/>
     </row>
-    <row r="55" spans="1:6" s="1" customFormat="1" ht="28">
+    <row r="55" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="9">
         <v>4</v>
       </c>
@@ -4594,7 +4596,7 @@
       <c r="E55" s="52"/>
       <c r="F55" s="26"/>
     </row>
-    <row r="56" spans="1:6" ht="28">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
         <v>5</v>
       </c>
@@ -4607,7 +4609,7 @@
       <c r="D56" s="33"/>
       <c r="E56" s="38"/>
     </row>
-    <row r="57" spans="1:6" ht="15">
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
         <v>6</v>
       </c>
@@ -4620,12 +4622,12 @@
       <c r="D57" s="33"/>
       <c r="E57" s="43"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="64"/>
     </row>
-    <row r="59" spans="1:6" s="1" customFormat="1" ht="23">
+    <row r="59" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A59" s="23" t="s">
         <v>85</v>
       </c>
@@ -4642,7 +4644,7 @@
       </c>
       <c r="F59" s="26"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>0</v>
       </c>
@@ -4659,7 +4661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="28">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
         <v>1</v>
       </c>
@@ -4671,10 +4673,10 @@
       </c>
       <c r="D61" s="33"/>
       <c r="E61" s="38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="9">
         <v>2</v>
       </c>
@@ -4687,22 +4689,22 @@
       <c r="D62" s="33"/>
       <c r="E62" s="38"/>
     </row>
-    <row r="63" spans="1:6" ht="15">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="9">
         <v>3</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C63" s="38">
         <v>5</v>
       </c>
       <c r="D63" s="33"/>
       <c r="E63" s="38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
         <v>4</v>
       </c>
@@ -4715,22 +4717,20 @@
       <c r="D64" s="33"/>
       <c r="E64" s="38"/>
     </row>
-    <row r="65" spans="1:6" ht="15">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
         <v>5</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C65" s="38">
         <v>5</v>
       </c>
       <c r="D65" s="33"/>
-      <c r="E65" s="38" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15">
+      <c r="E65" s="38"/>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
         <v>6</v>
       </c>
@@ -4743,12 +4743,12 @@
       <c r="D66" s="33"/>
       <c r="E66" s="38"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="64"/>
     </row>
-    <row r="68" spans="1:6" s="1" customFormat="1" ht="23">
+    <row r="68" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A68" s="23" t="s">
         <v>73</v>
       </c>
@@ -4764,7 +4764,7 @@
       </c>
       <c r="F68" s="26"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>0</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15">
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
         <v>1</v>
       </c>
@@ -4794,7 +4794,7 @@
       <c r="D70" s="33"/>
       <c r="E70" s="38"/>
     </row>
-    <row r="71" spans="1:6" ht="15">
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
         <v>2</v>
       </c>
@@ -4805,11 +4805,9 @@
         <v>5</v>
       </c>
       <c r="D71" s="33"/>
-      <c r="E71" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15">
+      <c r="E71" s="38"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="9">
         <v>3</v>
       </c>
@@ -4822,7 +4820,7 @@
       <c r="D72" s="33"/>
       <c r="E72" s="38"/>
     </row>
-    <row r="73" spans="1:6" ht="15">
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="9">
         <v>4</v>
       </c>
@@ -4835,12 +4833,12 @@
       <c r="D73" s="33"/>
       <c r="E73" s="38"/>
     </row>
-    <row r="74" spans="1:6" ht="15">
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>5</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C74" s="34">
         <v>5</v>
@@ -4848,17 +4846,17 @@
       <c r="D74" s="33"/>
       <c r="E74" s="38"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="64"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="64"/>
     </row>
-    <row r="77" spans="1:6" s="1" customFormat="1" ht="23">
+    <row r="77" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A77" s="23" t="s">
         <v>74</v>
       </c>
@@ -4874,7 +4872,7 @@
       </c>
       <c r="F77" s="26"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>0</v>
       </c>
@@ -4891,7 +4889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15">
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
         <v>1</v>
       </c>
@@ -4904,7 +4902,7 @@
       <c r="D79" s="33"/>
       <c r="E79" s="38"/>
     </row>
-    <row r="80" spans="1:6" ht="15">
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
         <v>2</v>
       </c>
@@ -4917,12 +4915,12 @@
       <c r="D80" s="33"/>
       <c r="E80" s="38"/>
     </row>
-    <row r="81" spans="1:6" ht="15">
+    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>3</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C81" s="34">
         <v>5</v>
@@ -4930,7 +4928,7 @@
       <c r="D81" s="33"/>
       <c r="E81" s="38"/>
     </row>
-    <row r="82" spans="1:6" ht="28">
+    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>4</v>
       </c>
@@ -4943,7 +4941,7 @@
       <c r="D82" s="33"/>
       <c r="E82" s="38"/>
     </row>
-    <row r="83" spans="1:6" ht="15">
+    <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
         <v>5</v>
       </c>
@@ -4956,14 +4954,14 @@
       <c r="D83" s="33"/>
       <c r="E83" s="38"/>
     </row>
-    <row r="85" spans="1:6" s="1" customFormat="1">
+    <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
       <c r="E85" s="66"/>
       <c r="F85" s="26"/>
     </row>
-    <row r="86" spans="1:6" ht="23">
+    <row r="86" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A86" s="23" t="s">
         <v>75</v>
       </c>
@@ -4979,7 +4977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>0</v>
       </c>
@@ -4996,7 +4994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="15">
+    <row r="88" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
         <v>1</v>
       </c>
@@ -5009,12 +5007,12 @@
       <c r="D88" s="33"/>
       <c r="E88" s="38"/>
     </row>
-    <row r="89" spans="1:6" ht="15">
+    <row r="89" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
         <v>2</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C89" s="38">
         <v>5</v>
@@ -5022,12 +5020,12 @@
       <c r="D89" s="33"/>
       <c r="E89" s="38"/>
     </row>
-    <row r="90" spans="1:6" ht="15">
+    <row r="90" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="9">
         <v>3</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C90" s="38">
         <v>5</v>
@@ -5035,7 +5033,7 @@
       <c r="D90" s="33"/>
       <c r="E90" s="38"/>
     </row>
-    <row r="91" spans="1:6" ht="15">
+    <row r="91" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>4</v>
       </c>
@@ -5048,12 +5046,12 @@
       <c r="D91" s="33"/>
       <c r="E91" s="38"/>
     </row>
-    <row r="92" spans="1:6" ht="15">
+    <row r="92" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
         <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C92" s="38">
         <v>5</v>
@@ -5061,7 +5059,7 @@
       <c r="D92" s="33"/>
       <c r="E92" s="38"/>
     </row>
-    <row r="93" spans="1:6" ht="15">
+    <row r="93" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
         <v>6</v>
       </c>
@@ -5074,14 +5072,14 @@
       <c r="D93" s="33"/>
       <c r="E93" s="38"/>
     </row>
-    <row r="94" spans="1:6" s="1" customFormat="1">
+    <row r="94" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
       <c r="E94" s="66"/>
       <c r="F94" s="26"/>
     </row>
-    <row r="95" spans="1:6" ht="23">
+    <row r="95" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A95" s="23" t="s">
         <v>76</v>
       </c>
@@ -5097,7 +5095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>0</v>
       </c>
@@ -5114,7 +5112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="15">
+    <row r="97" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
         <v>1</v>
       </c>
@@ -5127,12 +5125,12 @@
       <c r="D97" s="33"/>
       <c r="E97" s="38"/>
     </row>
-    <row r="98" spans="1:6" ht="15">
+    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
         <v>2</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C98" s="34">
         <v>5</v>
@@ -5140,12 +5138,12 @@
       <c r="D98" s="33"/>
       <c r="E98" s="38"/>
     </row>
-    <row r="99" spans="1:6" ht="15">
+    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
         <v>3</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C99" s="34">
         <v>5</v>
@@ -5153,12 +5151,12 @@
       <c r="D99" s="33"/>
       <c r="E99" s="38"/>
     </row>
-    <row r="100" spans="1:6" ht="15">
+    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
         <v>4</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C100" s="34">
         <v>5</v>
@@ -5166,12 +5164,12 @@
       <c r="D100" s="33"/>
       <c r="E100" s="38"/>
     </row>
-    <row r="101" spans="1:6" ht="15">
+    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>5</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C101" s="34">
         <v>0</v>
@@ -5179,7 +5177,7 @@
       <c r="D101" s="33"/>
       <c r="E101" s="38"/>
     </row>
-    <row r="102" spans="1:6" ht="15">
+    <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>6</v>
       </c>
@@ -5192,7 +5190,7 @@
       <c r="D102" s="33"/>
       <c r="E102" s="38"/>
     </row>
-    <row r="103" spans="1:6" ht="15">
+    <row r="103" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>7</v>
       </c>
@@ -5204,15 +5202,15 @@
       </c>
       <c r="D103" s="33"/>
       <c r="E103" s="38" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="15">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>8</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C104" s="34">
         <v>5</v>
@@ -5220,14 +5218,14 @@
       <c r="D104" s="33"/>
       <c r="E104" s="38"/>
     </row>
-    <row r="105" spans="1:6" s="1" customFormat="1" ht="15">
+    <row r="105" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B105" s="55"/>
       <c r="C105" s="34"/>
       <c r="D105" s="56"/>
       <c r="E105" s="67"/>
       <c r="F105" s="26"/>
     </row>
-    <row r="106" spans="1:6" ht="23">
+    <row r="106" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A106" s="23" t="s">
         <v>77</v>
       </c>
@@ -5243,7 +5241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>0</v>
       </c>
@@ -5260,7 +5258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="15">
+    <row r="108" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="5">
         <v>1</v>
       </c>
@@ -5273,7 +5271,7 @@
       <c r="D108" s="33"/>
       <c r="E108" s="38"/>
     </row>
-    <row r="109" spans="1:6" ht="15">
+    <row r="109" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="5">
         <v>2</v>
       </c>
@@ -5286,12 +5284,12 @@
       <c r="D109" s="33"/>
       <c r="E109" s="65"/>
     </row>
-    <row r="110" spans="1:6" ht="15">
+    <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
         <v>3</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C110" s="34">
         <v>5</v>
@@ -5299,12 +5297,12 @@
       <c r="D110" s="33"/>
       <c r="E110" s="38"/>
     </row>
-    <row r="111" spans="1:6" ht="15">
+    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>4</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C111" s="34">
         <v>5</v>
@@ -5312,14 +5310,14 @@
       <c r="D111" s="33"/>
       <c r="E111" s="38"/>
     </row>
-    <row r="112" spans="1:6" s="1" customFormat="1" ht="15">
+    <row r="112" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B112" s="55"/>
       <c r="C112" s="34"/>
       <c r="D112" s="56"/>
       <c r="E112" s="67"/>
       <c r="F112" s="26"/>
     </row>
-    <row r="113" spans="1:6" ht="23">
+    <row r="113" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A113" s="23" t="s">
         <v>95</v>
       </c>
@@ -5335,7 +5333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>0</v>
       </c>
@@ -5352,7 +5350,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15">
+    <row r="115" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>1</v>
       </c>
@@ -5365,12 +5363,12 @@
       <c r="D115" s="33"/>
       <c r="E115" s="38"/>
     </row>
-    <row r="116" spans="1:6" ht="15">
+    <row r="116" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>2</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C116" s="34">
         <v>5</v>
@@ -5378,7 +5376,7 @@
       <c r="D116" s="33"/>
       <c r="E116" s="38"/>
     </row>
-    <row r="117" spans="1:6" ht="15">
+    <row r="117" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="5">
         <v>3</v>
       </c>
@@ -5391,7 +5389,7 @@
       <c r="D117" s="33"/>
       <c r="E117" s="38"/>
     </row>
-    <row r="118" spans="1:6" ht="15">
+    <row r="118" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="9">
         <v>4</v>
       </c>
@@ -5404,7 +5402,7 @@
       <c r="D118" s="33"/>
       <c r="E118" s="38"/>
     </row>
-    <row r="119" spans="1:6" ht="15">
+    <row r="119" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="9">
         <v>5</v>
       </c>
@@ -5417,12 +5415,12 @@
       <c r="D119" s="33"/>
       <c r="E119" s="38"/>
     </row>
-    <row r="120" spans="1:6" ht="15">
+    <row r="120" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>6</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C120" s="34">
         <v>5</v>
@@ -5430,7 +5428,7 @@
       <c r="D120" s="33"/>
       <c r="E120" s="38"/>
     </row>
-    <row r="121" spans="1:6" ht="15">
+    <row r="121" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="5">
         <v>7</v>
       </c>
@@ -5443,12 +5441,12 @@
       <c r="D121" s="33"/>
       <c r="E121" s="38"/>
     </row>
-    <row r="122" spans="1:6" ht="15">
+    <row r="122" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="5">
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C122" s="34">
         <v>5</v>
@@ -5456,14 +5454,14 @@
       <c r="D122" s="33"/>
       <c r="E122" s="38"/>
     </row>
-    <row r="123" spans="1:6" s="1" customFormat="1">
+    <row r="123" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="66"/>
       <c r="F123" s="26"/>
     </row>
-    <row r="124" spans="1:6" ht="23">
+    <row r="124" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A124" s="23" t="s">
         <v>78</v>
       </c>
@@ -5479,7 +5477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="5" t="s">
         <v>0</v>
       </c>
@@ -5496,7 +5494,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="15">
+    <row r="126" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>1</v>
       </c>
@@ -5509,7 +5507,7 @@
       <c r="D126" s="33"/>
       <c r="E126" s="38"/>
     </row>
-    <row r="127" spans="1:6" ht="15">
+    <row r="127" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="5">
         <v>2</v>
       </c>
@@ -5522,12 +5520,12 @@
       <c r="D127" s="33"/>
       <c r="E127" s="38"/>
     </row>
-    <row r="128" spans="1:6" ht="28">
+    <row r="128" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="9">
         <v>3</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C128" s="34">
         <v>5</v>
@@ -5535,12 +5533,12 @@
       <c r="D128" s="33"/>
       <c r="E128" s="38"/>
     </row>
-    <row r="129" spans="1:6" ht="15">
+    <row r="129" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="9">
         <v>4</v>
       </c>
       <c r="B129" s="55" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C129" s="34">
         <v>5</v>
@@ -5548,7 +5546,7 @@
       <c r="D129" s="33"/>
       <c r="E129" s="38"/>
     </row>
-    <row r="130" spans="1:6" ht="15">
+    <row r="130" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="9">
         <v>5</v>
       </c>
@@ -5560,15 +5558,15 @@
       </c>
       <c r="D130" s="33"/>
       <c r="E130" s="38" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="5">
         <v>6</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C131" s="34">
         <v>5</v>
@@ -5576,7 +5574,7 @@
       <c r="D131" s="33"/>
       <c r="E131" s="38"/>
     </row>
-    <row r="132" spans="1:6" ht="28">
+    <row r="132" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="5">
         <v>7</v>
       </c>
@@ -5589,12 +5587,12 @@
       <c r="D132" s="33"/>
       <c r="E132" s="38"/>
     </row>
-    <row r="133" spans="1:6" ht="15">
+    <row r="133" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="5">
         <v>8</v>
       </c>
       <c r="B133" s="55" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C133" s="34">
         <v>5</v>
@@ -5602,7 +5600,7 @@
       <c r="D133" s="33"/>
       <c r="E133" s="38"/>
     </row>
-    <row r="134" spans="1:6" ht="15">
+    <row r="134" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A134" s="9">
         <v>9</v>
       </c>
@@ -5615,12 +5613,12 @@
       <c r="D134" s="33"/>
       <c r="E134" s="38"/>
     </row>
-    <row r="135" spans="1:6" ht="15">
+    <row r="135" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="26">
         <v>10</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C135" s="34">
         <v>5</v>
@@ -5628,14 +5626,14 @@
       <c r="D135" s="33"/>
       <c r="E135" s="38"/>
     </row>
-    <row r="136" spans="1:6" s="1" customFormat="1">
+    <row r="136" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B136"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="66"/>
       <c r="F136" s="26"/>
     </row>
-    <row r="137" spans="1:6" ht="23">
+    <row r="137" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A137" s="23" t="s">
         <v>79</v>
       </c>
@@ -5651,7 +5649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:6">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>0</v>
       </c>
@@ -5668,7 +5666,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:6" ht="15">
+    <row r="139" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="5">
         <v>1</v>
       </c>
@@ -5681,7 +5679,7 @@
       <c r="D139" s="33"/>
       <c r="E139" s="38"/>
     </row>
-    <row r="140" spans="1:6" ht="15">
+    <row r="140" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="9">
         <v>2</v>
       </c>
@@ -5694,7 +5692,7 @@
       <c r="D140" s="33"/>
       <c r="E140" s="38"/>
     </row>
-    <row r="141" spans="1:6" ht="15">
+    <row r="141" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="9">
         <v>3</v>
       </c>
@@ -5707,7 +5705,7 @@
       <c r="D141" s="33"/>
       <c r="E141" s="38"/>
     </row>
-    <row r="142" spans="1:6" ht="15">
+    <row r="142" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="9">
         <v>4</v>
       </c>
@@ -5720,12 +5718,12 @@
       <c r="D142" s="33"/>
       <c r="E142" s="38"/>
     </row>
-    <row r="143" spans="1:6" ht="15">
+    <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>6</v>
       </c>
       <c r="B143" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C143" s="34">
         <v>3</v>
@@ -5733,12 +5731,12 @@
       <c r="D143" s="33"/>
       <c r="E143" s="38"/>
     </row>
-    <row r="144" spans="1:6" ht="15">
+    <row r="144" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>7</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C144" s="34">
         <v>5</v>
@@ -5746,7 +5744,7 @@
       <c r="D144" s="33"/>
       <c r="E144" s="38"/>
     </row>
-    <row r="145" spans="1:6" ht="15">
+    <row r="145" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>8</v>
       </c>
@@ -5759,19 +5757,19 @@
       <c r="D145" s="33"/>
       <c r="E145" s="38"/>
     </row>
-    <row r="146" spans="1:6">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="64"/>
     </row>
-    <row r="147" spans="1:6" s="1" customFormat="1">
+    <row r="147" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="66"/>
       <c r="F147" s="26"/>
     </row>
-    <row r="148" spans="1:6" ht="23">
+    <row r="148" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A148" s="23" t="s">
         <v>80</v>
       </c>
@@ -5787,7 +5785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:6">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="5" t="s">
         <v>0</v>
       </c>
@@ -5804,7 +5802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15">
+    <row r="150" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="20">
         <v>1</v>
       </c>
@@ -5817,7 +5815,7 @@
       <c r="D150" s="33"/>
       <c r="E150" s="38"/>
     </row>
-    <row r="151" spans="1:6" ht="15">
+    <row r="151" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="5">
         <v>2</v>
       </c>
@@ -5829,10 +5827,10 @@
       </c>
       <c r="D151" s="33"/>
       <c r="E151" s="38" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="5">
         <v>3</v>
       </c>
@@ -5845,7 +5843,7 @@
       <c r="D152" s="33"/>
       <c r="E152" s="38"/>
     </row>
-    <row r="153" spans="1:6" ht="15">
+    <row r="153" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="9">
         <v>4</v>
       </c>
@@ -5858,12 +5856,12 @@
       <c r="D153" s="33"/>
       <c r="E153" s="38"/>
     </row>
-    <row r="154" spans="1:6" ht="15">
+    <row r="154" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="9">
         <v>5</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C154" s="34">
         <v>5</v>
@@ -5871,12 +5869,12 @@
       <c r="D154" s="33"/>
       <c r="E154" s="38"/>
     </row>
-    <row r="155" spans="1:6" ht="28">
+    <row r="155" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>6</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C155" s="34">
         <v>5</v>
@@ -5884,7 +5882,7 @@
       <c r="D155" s="33"/>
       <c r="E155" s="52"/>
     </row>
-    <row r="156" spans="1:6" ht="15">
+    <row r="156" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
         <v>7</v>
       </c>
@@ -5896,25 +5894,25 @@
       </c>
       <c r="D156" s="33"/>
       <c r="E156" s="38" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="28">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="9">
         <v>8</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C157" s="34">
         <v>5</v>
       </c>
       <c r="D157" s="33"/>
       <c r="E157" s="38" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A158" s="9">
         <v>9</v>
       </c>
@@ -5927,12 +5925,12 @@
       <c r="D158" s="33"/>
       <c r="E158" s="52"/>
     </row>
-    <row r="159" spans="1:6" ht="15">
+    <row r="159" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
         <v>10</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C159" s="34">
         <v>5</v>
@@ -5940,7 +5938,7 @@
       <c r="D159" s="33"/>
       <c r="E159" s="38"/>
     </row>
-    <row r="160" spans="1:6" ht="15">
+    <row r="160" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="20">
         <v>11</v>
       </c>
@@ -5953,12 +5951,12 @@
       <c r="D160" s="33"/>
       <c r="E160" s="38"/>
     </row>
-    <row r="161" spans="1:5" ht="15">
+    <row r="161" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="59">
         <v>12</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C161" s="34">
         <v>5</v>
@@ -5966,12 +5964,12 @@
       <c r="D161" s="33"/>
       <c r="E161" s="38"/>
     </row>
-    <row r="162" spans="1:5" ht="15">
+    <row r="162" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="26">
         <v>13</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C162" s="34">
         <v>5</v>
@@ -5979,12 +5977,12 @@
       <c r="D162" s="33"/>
       <c r="E162" s="38"/>
     </row>
-    <row r="163" spans="1:5" ht="15">
+    <row r="163" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="26">
         <v>14</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C163" s="34">
         <v>5</v>
@@ -5992,12 +5990,12 @@
       <c r="D163" s="33"/>
       <c r="E163" s="38"/>
     </row>
-    <row r="164" spans="1:5">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="64"/>
     </row>
-    <row r="165" spans="1:5" ht="23">
+    <row r="165" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A165" s="23" t="s">
         <v>81</v>
       </c>
@@ -6013,7 +6011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:5">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="5" t="s">
         <v>0</v>
       </c>
@@ -6030,7 +6028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="15">
+    <row r="167" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="5">
         <v>1</v>
       </c>
@@ -6042,15 +6040,15 @@
       </c>
       <c r="D167" s="33"/>
       <c r="E167" s="38" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" ht="15">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="5">
         <v>2</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C168" s="34">
         <v>0</v>
@@ -6058,7 +6056,7 @@
       <c r="D168" s="33"/>
       <c r="E168" s="38"/>
     </row>
-    <row r="169" spans="1:5" ht="15">
+    <row r="169" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="5">
         <v>3</v>
       </c>
@@ -6071,12 +6069,12 @@
       <c r="D169" s="33"/>
       <c r="E169" s="38"/>
     </row>
-    <row r="170" spans="1:5" ht="15">
+    <row r="170" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="9">
         <v>4</v>
       </c>
       <c r="B170" s="55" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C170" s="34">
         <v>0</v>
@@ -6084,17 +6082,17 @@
       <c r="D170" s="33"/>
       <c r="E170" s="38"/>
     </row>
-    <row r="171" spans="1:5">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="64"/>
     </row>
-    <row r="172" spans="1:5" ht="23">
+    <row r="172" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A172" s="23" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B172" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C172" s="7"/>
       <c r="D172" s="28" t="s">
@@ -6105,7 +6103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:5">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="5" t="s">
         <v>0</v>
       </c>
@@ -6122,12 +6120,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="15">
+    <row r="174" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="5">
         <v>1</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C174" s="34">
         <v>5</v>
@@ -6135,12 +6133,12 @@
       <c r="D174" s="33"/>
       <c r="E174" s="38"/>
     </row>
-    <row r="175" spans="1:5" ht="15">
+    <row r="175" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="5">
         <v>2</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C175" s="34">
         <v>5</v>
@@ -6148,12 +6146,12 @@
       <c r="D175" s="33"/>
       <c r="E175" s="38"/>
     </row>
-    <row r="176" spans="1:5" ht="15">
+    <row r="176" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>3</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C176" s="34">
         <v>5</v>
@@ -6161,16 +6159,16 @@
       <c r="D176" s="33"/>
       <c r="E176" s="38"/>
     </row>
-    <row r="178" spans="1:6" s="54" customFormat="1" ht="28">
+    <row r="178" spans="1:6" s="54" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A178" s="53" t="s">
         <v>93</v>
       </c>
       <c r="E178" s="68"/>
       <c r="F178" s="74" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="23">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A179" s="24" t="s">
         <v>82</v>
       </c>
@@ -6189,10 +6187,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" ht="18">
+    <row r="180" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F180" s="74"/>
     </row>
-    <row r="181" spans="1:6" ht="18">
+    <row r="181" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A181" s="49" t="s">
         <v>83</v>
       </c>
@@ -6211,7 +6209,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="1:6" ht="18">
+    <row r="182" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A182" s="49" t="s">
         <v>84</v>
       </c>
@@ -6230,7 +6228,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="1:6" ht="18">
+    <row r="183" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A183" s="49" t="s">
         <v>85</v>
       </c>
@@ -6249,7 +6247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="1:6" ht="23">
+    <row r="184" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A184" s="48">
         <v>2</v>
       </c>
@@ -6264,10 +6262,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:6" ht="18">
+    <row r="185" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F185" s="74"/>
     </row>
-    <row r="186" spans="1:6" ht="18">
+    <row r="186" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A186" s="49" t="s">
         <v>73</v>
       </c>
@@ -6286,7 +6284,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="187" spans="1:6" ht="18">
+    <row r="187" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A187" s="49" t="s">
         <v>74</v>
       </c>
@@ -6305,7 +6303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:6" ht="18">
+    <row r="188" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A188" s="49" t="s">
         <v>75</v>
       </c>
@@ -6324,7 +6322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:6" ht="18">
+    <row r="189" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A189" s="49" t="s">
         <v>76</v>
       </c>
@@ -6343,7 +6341,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="190" spans="1:6" ht="18">
+    <row r="190" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A190" s="49" t="s">
         <v>77</v>
       </c>
@@ -6362,7 +6360,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="191" spans="1:6" ht="18">
+    <row r="191" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A191" s="49" t="s">
         <v>95</v>
       </c>
@@ -6381,7 +6379,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="192" spans="1:6" ht="18">
+    <row r="192" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A192" s="49" t="s">
         <v>78</v>
       </c>
@@ -6400,7 +6398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="193" spans="1:6" ht="18">
+    <row r="193" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A193" s="49" t="s">
         <v>79</v>
       </c>
@@ -6419,7 +6417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:6" ht="18">
+    <row r="194" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A194" s="49" t="s">
         <v>80</v>
       </c>
@@ -6438,7 +6436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:6" ht="18">
+    <row r="195" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A195" s="49" t="s">
         <v>81</v>
       </c>
@@ -6456,12 +6454,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:6" ht="18">
+    <row r="196" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A196" s="49" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B196" s="10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C196" s="51"/>
       <c r="D196" s="50" t="s">
@@ -6475,7 +6473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="197" spans="1:6" ht="23">
+    <row r="197" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A197" s="48">
         <v>3</v>
       </c>
@@ -6490,15 +6488,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:6" ht="18">
+    <row r="198" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F198" s="74"/>
     </row>
-    <row r="199" spans="1:6" ht="18">
+    <row r="199" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F199" s="74"/>
     </row>
-    <row r="200" spans="1:6" ht="20">
+    <row r="200" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B200" s="48" t="s">
-        <v>98</v>
+        <v>180</v>
       </c>
       <c r="E200" s="77">
         <f>((E179*F179)+E184*F184+E197*F197)/(F179+F184+F197)</f>
@@ -6506,19 +6504,19 @@
       </c>
       <c r="F200" s="74"/>
     </row>
-    <row r="205" spans="1:6">
+    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="206" spans="1:6">
-      <c r="A206" s="1" t="s">
+    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A207" s="1" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6">
-      <c r="A207" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -6559,7 +6557,7 @@
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6579,16 +6577,16 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refs #736 Nutzwertanalyse Monitorkonstellation
Former-commit-id: 9ecad9682ac864c06ecc8d3e7b562c73548c946a
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
+++ b/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
@@ -3826,8 +3826,8 @@
   </sheetPr>
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B201" sqref="B201"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,7 +3975,9 @@
       </c>
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10" s="72"/>
+      <c r="F10" s="73">
+        <v>40991</v>
+      </c>
     </row>
     <row r="11" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A11" s="9">

</xml_diff>

<commit_message>
refs #677 Kriterienliste angepasst
Former-commit-id: 00ae7b05ec016ebc4033561c6af54be859ddbe42
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
+++ b/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="183">
   <si>
     <t>#</t>
   </si>
@@ -620,13 +620,20 @@
     <t>Screenshot in Dokumentation</t>
   </si>
   <si>
-    <t>Übernahme aus SA</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>Gesamtnote</t>
+  </si>
+  <si>
+    <t>Übernahme aus SA, 23.04.2012</t>
+  </si>
+  <si>
+    <t>Zusammen entschieden, dass vollständiges Backlog nicht möglich
+=&gt; Bei jeweiligem Sprint werden nächste Elemente priorisiert</t>
+  </si>
+  <si>
+    <t>Für jeweiligen Sprint am Meeting realisierte User Stories werden kontrolliert; nächste User Stories werden abgenommen</t>
   </si>
 </sst>
 </file>
@@ -636,7 +643,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,12 +712,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -738,18 +747,21 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF505050"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -757,6 +769,7 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -764,6 +777,7 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -771,18 +785,21 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -802,18 +819,34 @@
       <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF505050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -976,7 +1009,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1091,9 +1124,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1179,6 +1209,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="131">
@@ -1317,6 +1351,37 @@
   <dxfs count="121">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1331,7 +1396,524 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1362,670 +1944,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2057,6 +1975,37 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2108,7 +2057,62 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2140,6 +2144,36 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3341,48 +3375,34 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F34" totalsRowCount="1" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48">
   <autoFilter ref="A4:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="47" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="46" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="G" dataDxfId="45" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="N" dataDxfId="44" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="43" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="besprochen am" dataDxfId="42" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="G" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="3" name="N" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="5" name="besprochen am" dataDxfId="37" totalsRowDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:E93" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:E93" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A87:E93"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="38"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="37"/>
-    <tableColumn id="5" name="G" dataDxfId="36"/>
-    <tableColumn id="3" name="N" dataDxfId="35"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="34"/>
+    <tableColumn id="1" name="#" dataDxfId="32"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="31"/>
+    <tableColumn id="5" name="G" dataDxfId="30"/>
+    <tableColumn id="3" name="N" dataDxfId="29"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:E83" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:E83" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
   <autoFilter ref="A78:E83"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="30"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="29"/>
-    <tableColumn id="5" name="G" dataDxfId="28"/>
-    <tableColumn id="3" name="N" dataDxfId="27"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="26"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E145" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A138:E145"/>
   <tableColumns count="5">
     <tableColumn id="1" name="#" dataDxfId="24"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="23"/>
@@ -3394,9 +3414,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A125:E135"/>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E145" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A138:E145"/>
   <tableColumns count="5">
     <tableColumn id="1" name="#" dataDxfId="18"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="17"/>
@@ -3408,15 +3428,29 @@
 </table>
 </file>
 
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A125:E135"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="#" dataDxfId="12"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="11"/>
+    <tableColumn id="5" name="G" dataDxfId="10"/>
+    <tableColumn id="3" name="N" dataDxfId="9"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table152" displayName="Table152" ref="A173:E176" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table152" displayName="Table152" ref="A173:E176" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A173:E176"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="10"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="9"/>
-    <tableColumn id="5" name="G" dataDxfId="8"/>
-    <tableColumn id="3" name="N" dataDxfId="7"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="6"/>
+    <tableColumn id="1" name="#" dataDxfId="4"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="3"/>
+    <tableColumn id="5" name="G" dataDxfId="2"/>
+    <tableColumn id="3" name="N" dataDxfId="1"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3826,8 +3860,8 @@
   </sheetPr>
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3836,21 +3870,21 @@
     <col min="2" max="2" width="120.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" style="60" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="71" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" style="59" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="70" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="61"/>
-      <c r="F1" s="71"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="70"/>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="3"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="71"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="70"/>
     </row>
     <row r="3" spans="1:6" s="18" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="24" t="s">
@@ -3863,11 +3897,11 @@
       <c r="D3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="62">
+      <c r="E3" s="61">
         <f>SUMPRODUCT(Table2[G],Table2[N])/SUM(Table2[G])</f>
         <v>0</v>
       </c>
-      <c r="F3" s="71"/>
+      <c r="F3" s="70"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A4" s="29" t="s">
@@ -3901,7 +3935,7 @@
       </c>
       <c r="D5"/>
       <c r="E5"/>
-      <c r="F5" s="72"/>
+      <c r="F5" s="71"/>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A6" s="31">
@@ -3915,7 +3949,7 @@
       </c>
       <c r="D6"/>
       <c r="E6"/>
-      <c r="F6" s="72"/>
+      <c r="F6" s="71"/>
     </row>
     <row r="7" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A7" s="31">
@@ -3929,7 +3963,7 @@
       </c>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7" s="72"/>
+      <c r="F7" s="71"/>
     </row>
     <row r="8" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A8" s="5">
@@ -3943,8 +3977,8 @@
       </c>
       <c r="D8"/>
       <c r="E8"/>
-      <c r="F8" s="73" t="s">
-        <v>178</v>
+      <c r="F8" s="72" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -3959,8 +3993,8 @@
       </c>
       <c r="D9"/>
       <c r="E9"/>
-      <c r="F9" s="72" t="s">
-        <v>179</v>
+      <c r="F9" s="71" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -3975,7 +4009,7 @@
       </c>
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10" s="73">
+      <c r="F10" s="72">
         <v>40991</v>
       </c>
     </row>
@@ -3991,7 +4025,9 @@
       </c>
       <c r="D11"/>
       <c r="E11"/>
-      <c r="F11" s="72"/>
+      <c r="F11" s="78">
+        <v>41022</v>
+      </c>
     </row>
     <row r="12" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A12" s="5">
@@ -4005,7 +4041,9 @@
       </c>
       <c r="D12"/>
       <c r="E12"/>
-      <c r="F12" s="72"/>
+      <c r="F12" s="78">
+        <v>41022</v>
+      </c>
     </row>
     <row r="13" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A13" s="5">
@@ -4019,7 +4057,9 @@
       </c>
       <c r="D13"/>
       <c r="E13"/>
-      <c r="F13" s="72"/>
+      <c r="F13" s="71" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A14" s="5">
@@ -4033,7 +4073,7 @@
       </c>
       <c r="D14"/>
       <c r="E14"/>
-      <c r="F14" s="72"/>
+      <c r="F14" s="71"/>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A15" s="9">
@@ -4047,7 +4087,9 @@
       </c>
       <c r="D15"/>
       <c r="E15"/>
-      <c r="F15" s="72"/>
+      <c r="F15" s="71" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A16" s="9">
@@ -4061,7 +4103,7 @@
       </c>
       <c r="D16"/>
       <c r="E16"/>
-      <c r="F16" s="72"/>
+      <c r="F16" s="71"/>
     </row>
     <row r="17" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A17" s="5">
@@ -4075,7 +4117,7 @@
       </c>
       <c r="D17"/>
       <c r="E17"/>
-      <c r="F17" s="72"/>
+      <c r="F17" s="71"/>
     </row>
     <row r="18" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A18" s="5">
@@ -4089,7 +4131,9 @@
       </c>
       <c r="D18"/>
       <c r="E18"/>
-      <c r="F18" s="72"/>
+      <c r="F18" s="78">
+        <v>41022</v>
+      </c>
     </row>
     <row r="19" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A19" s="25">
@@ -4103,7 +4147,7 @@
       </c>
       <c r="D19"/>
       <c r="E19"/>
-      <c r="F19" s="72"/>
+      <c r="F19" s="71"/>
     </row>
     <row r="20" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A20" s="30">
@@ -4117,7 +4161,7 @@
       </c>
       <c r="D20"/>
       <c r="E20"/>
-      <c r="F20" s="72"/>
+      <c r="F20" s="71"/>
     </row>
     <row r="21" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A21" s="25">
@@ -4131,7 +4175,7 @@
       </c>
       <c r="D21"/>
       <c r="E21"/>
-      <c r="F21" s="72"/>
+      <c r="F21" s="71"/>
     </row>
     <row r="22" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A22" s="25">
@@ -4145,7 +4189,7 @@
       </c>
       <c r="D22"/>
       <c r="E22"/>
-      <c r="F22" s="72"/>
+      <c r="F22" s="71"/>
     </row>
     <row r="23" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A23" s="25">
@@ -4159,7 +4203,7 @@
       </c>
       <c r="D23"/>
       <c r="E23"/>
-      <c r="F23" s="72"/>
+      <c r="F23" s="71"/>
     </row>
     <row r="24" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A24" s="25">
@@ -4173,7 +4217,7 @@
       </c>
       <c r="D24"/>
       <c r="E24"/>
-      <c r="F24" s="72"/>
+      <c r="F24" s="71"/>
     </row>
     <row r="25" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A25" s="25">
@@ -4187,20 +4231,20 @@
       </c>
       <c r="D25"/>
       <c r="E25"/>
-      <c r="F25" s="72"/>
+      <c r="F25" s="71"/>
     </row>
     <row r="26" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25">
         <v>22</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="77" t="s">
         <v>139</v>
       </c>
       <c r="C26" s="40">
         <v>5</v>
       </c>
       <c r="E26"/>
-      <c r="F26" s="72"/>
+      <c r="F26" s="71"/>
     </row>
     <row r="27" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A27" s="25">
@@ -4214,7 +4258,7 @@
       </c>
       <c r="D27"/>
       <c r="E27"/>
-      <c r="F27" s="72"/>
+      <c r="F27" s="71"/>
     </row>
     <row r="28" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A28" s="25">
@@ -4228,7 +4272,7 @@
       </c>
       <c r="D28"/>
       <c r="E28"/>
-      <c r="F28" s="72"/>
+      <c r="F28" s="71"/>
     </row>
     <row r="29" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A29" s="25">
@@ -4242,7 +4286,7 @@
       </c>
       <c r="D29"/>
       <c r="E29"/>
-      <c r="F29" s="72"/>
+      <c r="F29" s="71"/>
     </row>
     <row r="30" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A30" s="25">
@@ -4256,7 +4300,7 @@
       </c>
       <c r="D30" s="33"/>
       <c r="E30"/>
-      <c r="F30" s="72"/>
+      <c r="F30" s="71"/>
     </row>
     <row r="31" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A31" s="25">
@@ -4270,7 +4314,7 @@
       </c>
       <c r="D31" s="33"/>
       <c r="E31" s="43"/>
-      <c r="F31" s="72"/>
+      <c r="F31" s="71"/>
     </row>
     <row r="32" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A32" s="21">
@@ -4284,28 +4328,28 @@
       </c>
       <c r="D32" s="41"/>
       <c r="E32" s="42"/>
-      <c r="F32" s="72"/>
+      <c r="F32" s="71"/>
     </row>
     <row r="33" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A33" s="57">
+      <c r="A33" s="56">
         <v>29</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="57" t="s">
         <v>141</v>
       </c>
       <c r="C33" s="40">
         <v>5</v>
       </c>
       <c r="D33" s="44"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="72"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="71"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="15"/>
       <c r="C34" s="45"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="47"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="46"/>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A35" s="23" t="s">
@@ -4317,7 +4361,7 @@
       <c r="D35" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="62">
+      <c r="E35" s="61">
         <f>SUMPRODUCT(Table6[G],Table6[N])/SUM(Table6[G])</f>
         <v>0</v>
       </c>
@@ -4351,10 +4395,10 @@
         <v>5</v>
       </c>
       <c r="D37" s="33"/>
-      <c r="E37" s="47" t="s">
+      <c r="E37" s="46" t="s">
         <v>143</v>
       </c>
-      <c r="F37" s="71"/>
+      <c r="F37" s="70"/>
     </row>
     <row r="38" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A38" s="12">
@@ -4368,7 +4412,7 @@
       </c>
       <c r="D38" s="33"/>
       <c r="E38" s="42"/>
-      <c r="F38" s="71"/>
+      <c r="F38" s="70"/>
     </row>
     <row r="39" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A39" s="12">
@@ -4384,7 +4428,7 @@
       <c r="E39" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="F39" s="71"/>
+      <c r="F39" s="70"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -4504,12 +4548,12 @@
       <c r="E48" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="F48" s="71"/>
+      <c r="F48" s="70"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
-      <c r="E49" s="64"/>
+      <c r="E49" s="63"/>
     </row>
     <row r="50" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A50" s="23" t="s">
@@ -4522,7 +4566,7 @@
       <c r="D50" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="62">
+      <c r="E50" s="61">
         <f>SUMPRODUCT(Table12[G],Table12[N])/SUM(Table12[G])</f>
         <v>0</v>
       </c>
@@ -4555,7 +4599,7 @@
         <v>5</v>
       </c>
       <c r="D52" s="33"/>
-      <c r="E52" s="65"/>
+      <c r="E52" s="64"/>
     </row>
     <row r="53" spans="1:6" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -4569,7 +4613,7 @@
       </c>
       <c r="D53" s="33"/>
       <c r="E53" s="38"/>
-      <c r="F53" s="71"/>
+      <c r="F53" s="70"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="9">
@@ -4595,7 +4639,7 @@
         <v>5</v>
       </c>
       <c r="D55" s="33"/>
-      <c r="E55" s="52"/>
+      <c r="E55" s="51"/>
       <c r="F55" s="26"/>
     </row>
     <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -4627,7 +4671,7 @@
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
-      <c r="E58" s="64"/>
+      <c r="E58" s="63"/>
     </row>
     <row r="59" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A59" s="23" t="s">
@@ -4640,7 +4684,7 @@
       <c r="D59" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E59" s="62">
+      <c r="E59" s="61">
         <f>SUMPRODUCT(Table3[G],Table3[N])/SUM(Table3[G])</f>
         <v>0</v>
       </c>
@@ -4748,7 +4792,7 @@
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
-      <c r="E67" s="64"/>
+      <c r="E67" s="63"/>
     </row>
     <row r="68" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A68" s="23" t="s">
@@ -4760,7 +4804,7 @@
       <c r="D68" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E68" s="62">
+      <c r="E68" s="61">
         <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
         <v>0</v>
       </c>
@@ -4851,12 +4895,12 @@
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="64"/>
+      <c r="E75" s="63"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="64"/>
+      <c r="E76" s="63"/>
     </row>
     <row r="77" spans="1:6" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A77" s="23" t="s">
@@ -4868,7 +4912,7 @@
       <c r="D77" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E77" s="62">
+      <c r="E77" s="61">
         <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
         <v>0</v>
       </c>
@@ -4960,7 +5004,7 @@
       <c r="B85"/>
       <c r="C85" s="7"/>
       <c r="D85" s="7"/>
-      <c r="E85" s="66"/>
+      <c r="E85" s="65"/>
       <c r="F85" s="26"/>
     </row>
     <row r="86" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -4974,7 +5018,7 @@
       <c r="D86" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E86" s="62">
+      <c r="E86" s="61">
         <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
         <v>0</v>
       </c>
@@ -5078,7 +5122,7 @@
       <c r="B94"/>
       <c r="C94" s="7"/>
       <c r="D94" s="7"/>
-      <c r="E94" s="66"/>
+      <c r="E94" s="65"/>
       <c r="F94" s="26"/>
     </row>
     <row r="95" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5092,7 +5136,7 @@
       <c r="D95" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E95" s="62">
+      <c r="E95" s="61">
         <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
         <v>0</v>
       </c>
@@ -5221,10 +5265,10 @@
       <c r="E104" s="38"/>
     </row>
     <row r="105" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B105" s="55"/>
+      <c r="B105" s="54"/>
       <c r="C105" s="34"/>
-      <c r="D105" s="56"/>
-      <c r="E105" s="67"/>
+      <c r="D105" s="55"/>
+      <c r="E105" s="66"/>
       <c r="F105" s="26"/>
     </row>
     <row r="106" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5238,7 +5282,7 @@
       <c r="D106" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E106" s="62">
+      <c r="E106" s="61">
         <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
         <v>0</v>
       </c>
@@ -5284,7 +5328,7 @@
         <v>5</v>
       </c>
       <c r="D109" s="33"/>
-      <c r="E109" s="65"/>
+      <c r="E109" s="64"/>
     </row>
     <row r="110" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="5">
@@ -5313,10 +5357,10 @@
       <c r="E111" s="38"/>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B112" s="55"/>
+      <c r="B112" s="54"/>
       <c r="C112" s="34"/>
-      <c r="D112" s="56"/>
-      <c r="E112" s="67"/>
+      <c r="D112" s="55"/>
+      <c r="E112" s="66"/>
       <c r="F112" s="26"/>
     </row>
     <row r="113" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5330,7 +5374,7 @@
       <c r="D113" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E113" s="62">
+      <c r="E113" s="61">
         <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
         <v>0</v>
       </c>
@@ -5460,7 +5504,7 @@
       <c r="B123"/>
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
-      <c r="E123" s="66"/>
+      <c r="E123" s="65"/>
       <c r="F123" s="26"/>
     </row>
     <row r="124" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5474,7 +5518,7 @@
       <c r="D124" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E124" s="62">
+      <c r="E124" s="61">
         <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
         <v>0</v>
       </c>
@@ -5539,7 +5583,7 @@
       <c r="A129" s="9">
         <v>4</v>
       </c>
-      <c r="B129" s="55" t="s">
+      <c r="B129" s="54" t="s">
         <v>123</v>
       </c>
       <c r="C129" s="34">
@@ -5593,7 +5637,7 @@
       <c r="A133" s="5">
         <v>8</v>
       </c>
-      <c r="B133" s="55" t="s">
+      <c r="B133" s="54" t="s">
         <v>176</v>
       </c>
       <c r="C133" s="34">
@@ -5632,7 +5676,7 @@
       <c r="B136"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
-      <c r="E136" s="66"/>
+      <c r="E136" s="65"/>
       <c r="F136" s="26"/>
     </row>
     <row r="137" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5646,7 +5690,7 @@
       <c r="D137" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E137" s="62">
+      <c r="E137" s="61">
         <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
         <v>0</v>
       </c>
@@ -5762,13 +5806,13 @@
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="64"/>
+      <c r="E146" s="63"/>
     </row>
     <row r="147" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B147"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="66"/>
+      <c r="E147" s="65"/>
       <c r="F147" s="26"/>
     </row>
     <row r="148" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -5782,7 +5826,7 @@
       <c r="D148" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E148" s="62">
+      <c r="E148" s="61">
         <f>SUMPRODUCT(Table10[G],Table10[N])/SUM(Table10[G])</f>
         <v>0</v>
       </c>
@@ -5882,7 +5926,7 @@
         <v>5</v>
       </c>
       <c r="D155" s="33"/>
-      <c r="E155" s="52"/>
+      <c r="E155" s="51"/>
     </row>
     <row r="156" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="9">
@@ -5925,7 +5969,7 @@
         <v>5</v>
       </c>
       <c r="D158" s="33"/>
-      <c r="E158" s="52"/>
+      <c r="E158" s="51"/>
     </row>
     <row r="159" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A159" s="9">
@@ -5954,7 +5998,7 @@
       <c r="E160" s="38"/>
     </row>
     <row r="161" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A161" s="59">
+      <c r="A161" s="58">
         <v>12</v>
       </c>
       <c r="B161" s="2" t="s">
@@ -5995,7 +6039,7 @@
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
-      <c r="E164" s="64"/>
+      <c r="E164" s="63"/>
     </row>
     <row r="165" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A165" s="23" t="s">
@@ -6008,7 +6052,7 @@
       <c r="D165" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E165" s="62">
+      <c r="E165" s="61">
         <f>SUMPRODUCT(Table15[G],Table15[N])/SUM(Table15[G])</f>
         <v>0</v>
       </c>
@@ -6075,7 +6119,7 @@
       <c r="A170" s="9">
         <v>4</v>
       </c>
-      <c r="B170" s="55" t="s">
+      <c r="B170" s="54" t="s">
         <v>119</v>
       </c>
       <c r="C170" s="34">
@@ -6087,7 +6131,7 @@
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
-      <c r="E171" s="64"/>
+      <c r="E171" s="63"/>
     </row>
     <row r="172" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A172" s="23" t="s">
@@ -6100,7 +6144,7 @@
       <c r="D172" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E172" s="62">
+      <c r="E172" s="61">
         <f>SUMPRODUCT(Table152[G],Table152[N])/SUM(Table152[G])</f>
         <v>0</v>
       </c>
@@ -6161,12 +6205,12 @@
       <c r="D176" s="33"/>
       <c r="E176" s="38"/>
     </row>
-    <row r="178" spans="1:6" s="54" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A178" s="53" t="s">
+    <row r="178" spans="1:6" s="53" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A178" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="E178" s="68"/>
-      <c r="F178" s="74" t="s">
+      <c r="E178" s="67"/>
+      <c r="F178" s="73" t="s">
         <v>152</v>
       </c>
     </row>
@@ -6181,330 +6225,330 @@
       <c r="D179" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E179" s="62">
+      <c r="E179" s="61">
         <f>SUMPRODUCT(Table2[G],Table2[N])/SUM(Table2[G])</f>
         <v>0</v>
       </c>
-      <c r="F179" s="74">
+      <c r="F179" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F180" s="74"/>
+      <c r="F180" s="73"/>
     </row>
     <row r="181" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A181" s="49" t="s">
+      <c r="A181" s="48" t="s">
         <v>83</v>
       </c>
       <c r="B181" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C181" s="10"/>
-      <c r="D181" s="50" t="s">
+      <c r="D181" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E181" s="69">
+      <c r="E181" s="68">
         <f>SUMPRODUCT(Table6[G],Table6[N])/SUM(Table6[G])</f>
         <v>0</v>
       </c>
-      <c r="F181" s="75">
+      <c r="F181" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="182" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A182" s="49" t="s">
+      <c r="A182" s="48" t="s">
         <v>84</v>
       </c>
       <c r="B182" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C182" s="10"/>
-      <c r="D182" s="50" t="s">
+      <c r="D182" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E182" s="69">
+      <c r="E182" s="68">
         <f>SUMPRODUCT(Table12[G],Table12[N])/SUM(Table12[G])</f>
         <v>0</v>
       </c>
-      <c r="F182" s="75">
+      <c r="F182" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="183" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A183" s="49" t="s">
+      <c r="A183" s="48" t="s">
         <v>85</v>
       </c>
       <c r="B183" s="10" t="s">
         <v>63</v>
       </c>
       <c r="C183" s="10"/>
-      <c r="D183" s="50" t="s">
+      <c r="D183" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E183" s="69">
+      <c r="E183" s="68">
         <f>SUMPRODUCT(Table3[G],Table3[N])/SUM(Table3[G])</f>
         <v>0</v>
       </c>
-      <c r="F183" s="75">
+      <c r="F183" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A184" s="48">
+      <c r="A184" s="47">
         <v>2</v>
       </c>
-      <c r="B184" s="76" t="s">
+      <c r="B184" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="E184" s="70">
+      <c r="E184" s="69">
         <f>SUMPRODUCT(F181:F183,E181:E183)/SUM(F181:F183)</f>
         <v>0</v>
       </c>
-      <c r="F184" s="74">
+      <c r="F184" s="73">
         <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F185" s="74"/>
+      <c r="F185" s="73"/>
     </row>
     <row r="186" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A186" s="49" t="s">
+      <c r="A186" s="48" t="s">
         <v>73</v>
       </c>
       <c r="B186" s="10" t="s">
         <v>70</v>
       </c>
       <c r="C186" s="10"/>
-      <c r="D186" s="50" t="s">
+      <c r="D186" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E186" s="69">
+      <c r="E186" s="68">
         <f>SUMPRODUCT(Table11[G],Table11[N])/SUM(Table11[G])</f>
         <v>0</v>
       </c>
-      <c r="F186" s="75">
+      <c r="F186" s="74">
         <v>4</v>
       </c>
     </row>
     <row r="187" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A187" s="49" t="s">
+      <c r="A187" s="48" t="s">
         <v>74</v>
       </c>
       <c r="B187" s="10" t="s">
         <v>64</v>
       </c>
       <c r="C187" s="10"/>
-      <c r="D187" s="50" t="s">
+      <c r="D187" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E187" s="69">
+      <c r="E187" s="68">
         <f>SUMPRODUCT(Table71518[G],Table71518[N])/SUM(Table71518[G])</f>
         <v>0</v>
       </c>
-      <c r="F187" s="75">
+      <c r="F187" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="188" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A188" s="49" t="s">
+      <c r="A188" s="48" t="s">
         <v>75</v>
       </c>
       <c r="B188" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C188" s="10"/>
-      <c r="D188" s="50" t="s">
+      <c r="D188" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E188" s="69">
+      <c r="E188" s="68">
         <f>SUMPRODUCT(Table715[G],Table715[N])/SUM(Table715[G])</f>
         <v>0</v>
       </c>
-      <c r="F188" s="75">
+      <c r="F188" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="189" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A189" s="49" t="s">
+      <c r="A189" s="48" t="s">
         <v>76</v>
       </c>
       <c r="B189" s="10" t="s">
         <v>69</v>
       </c>
       <c r="C189" s="10"/>
-      <c r="D189" s="50" t="s">
+      <c r="D189" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E189" s="69">
+      <c r="E189" s="68">
         <f>SUMPRODUCT(Table7[G],Table7[N])/SUM(Table7[G])</f>
         <v>0</v>
       </c>
-      <c r="F189" s="75">
+      <c r="F189" s="74">
         <v>6</v>
       </c>
     </row>
     <row r="190" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A190" s="49" t="s">
+      <c r="A190" s="48" t="s">
         <v>77</v>
       </c>
       <c r="B190" s="10" t="s">
         <v>96</v>
       </c>
       <c r="C190" s="10"/>
-      <c r="D190" s="50" t="s">
+      <c r="D190" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E190" s="69">
+      <c r="E190" s="68">
         <f>SUMPRODUCT(Table8[G],Table8[N])/SUM(Table8[G])</f>
         <v>0</v>
       </c>
-      <c r="F190" s="75">
+      <c r="F190" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="191" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A191" s="49" t="s">
+      <c r="A191" s="48" t="s">
         <v>95</v>
       </c>
       <c r="B191" s="10" t="s">
         <v>97</v>
       </c>
       <c r="C191" s="10"/>
-      <c r="D191" s="50" t="s">
+      <c r="D191" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E191" s="69">
+      <c r="E191" s="68">
         <f>SUMPRODUCT(Table9[G],Table9[N])/SUM(Table9[G])</f>
         <v>0</v>
       </c>
-      <c r="F191" s="75">
+      <c r="F191" s="74">
         <v>3</v>
       </c>
     </row>
     <row r="192" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A192" s="49" t="s">
+      <c r="A192" s="48" t="s">
         <v>78</v>
       </c>
       <c r="B192" s="10" t="s">
         <v>66</v>
       </c>
       <c r="C192" s="10"/>
-      <c r="D192" s="50" t="s">
+      <c r="D192" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E192" s="69">
+      <c r="E192" s="68">
         <f>SUMPRODUCT(Table1021[G],Table1021[N])/SUM(Table1021[G])</f>
         <v>0</v>
       </c>
-      <c r="F192" s="75">
+      <c r="F192" s="74">
         <v>6</v>
       </c>
     </row>
     <row r="193" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A193" s="49" t="s">
+      <c r="A193" s="48" t="s">
         <v>79</v>
       </c>
       <c r="B193" s="10" t="s">
         <v>67</v>
       </c>
       <c r="C193" s="10"/>
-      <c r="D193" s="50" t="s">
+      <c r="D193" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E193" s="69">
+      <c r="E193" s="68">
         <f>SUMPRODUCT(Table1020[G],Table1020[N])/SUM(Table1020[G])</f>
         <v>0</v>
       </c>
-      <c r="F193" s="75">
+      <c r="F193" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="194" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A194" s="49" t="s">
+      <c r="A194" s="48" t="s">
         <v>80</v>
       </c>
       <c r="B194" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C194" s="10"/>
-      <c r="D194" s="50" t="s">
+      <c r="D194" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E194" s="69">
+      <c r="E194" s="68">
         <f>SUMPRODUCT(Table10[G],Table10[N])/SUM(Table10[G])</f>
         <v>0</v>
       </c>
-      <c r="F194" s="75">
+      <c r="F194" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="195" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A195" s="49" t="s">
+      <c r="A195" s="48" t="s">
         <v>81</v>
       </c>
       <c r="B195" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C195" s="51"/>
-      <c r="D195" s="50" t="s">
+      <c r="C195" s="50"/>
+      <c r="D195" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E195" s="69">
+      <c r="E195" s="68">
         <v>0</v>
       </c>
-      <c r="F195" s="75">
+      <c r="F195" s="74">
         <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A196" s="49" t="s">
+      <c r="A196" s="48" t="s">
         <v>161</v>
       </c>
       <c r="B196" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C196" s="51"/>
-      <c r="D196" s="50" t="s">
+      <c r="C196" s="50"/>
+      <c r="D196" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E196" s="69">
+      <c r="E196" s="68">
         <f>E170</f>
         <v>0</v>
       </c>
-      <c r="F196" s="75">
+      <c r="F196" s="74">
         <v>2</v>
       </c>
     </row>
     <row r="197" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A197" s="48">
+      <c r="A197" s="47">
         <v>3</v>
       </c>
-      <c r="B197" s="76" t="s">
+      <c r="B197" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="E197" s="70">
+      <c r="E197" s="69">
         <f>SUMPRODUCT(F186:F196,E186:E196)/SUM(F186:F196)</f>
         <v>0</v>
       </c>
-      <c r="F197" s="74">
+      <c r="F197" s="73">
         <v>3</v>
       </c>
     </row>
     <row r="198" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F198" s="74"/>
+      <c r="F198" s="73"/>
     </row>
     <row r="199" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F199" s="74"/>
+      <c r="F199" s="73"/>
     </row>
     <row r="200" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="B200" s="48" t="s">
-        <v>180</v>
-      </c>
-      <c r="E200" s="77">
+      <c r="B200" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="E200" s="76">
         <f>((E179*F179)+E184*F184+E197*F197)/(F179+F184+F197)</f>
         <v>0</v>
       </c>
-      <c r="F200" s="74"/>
+      <c r="F200" s="73"/>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">

</xml_diff>

<commit_message>
refs #842 Update Kriterien SA-BA Stolze 2012 FS.xlsx
Former-commit-id: e7711f321a3a26fbc5bf62dcdf7bd807a45d31ce
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
+++ b/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15555" windowHeight="10995"/>
   </bookViews>
   <sheets>
     <sheet name="Leeres Kriterienblatt" sheetId="1" r:id="rId1"/>
@@ -3863,8 +3863,8 @@
   </sheetPr>
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B159" sqref="B159"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F196" sqref="F196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6194,7 +6194,7 @@
         <v>164</v>
       </c>
       <c r="C175" s="34">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D175" s="33"/>
       <c r="E175" s="38"/>
@@ -6504,7 +6504,7 @@
         <v>0</v>
       </c>
       <c r="F195" s="74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
refs #842 Kriterien z.T. übernommen
Former-commit-id: 2afbb6bb90c2d5d048db6bbf806f7f91ecea421c
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
+++ b/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15555" windowHeight="10995"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
   <si>
     <t>#</t>
   </si>
@@ -637,6 +637,22 @@
   </si>
   <si>
     <t>11.5.2012: Auf 0 setzen</t>
+  </si>
+  <si>
+    <t>geplant für sp13</t>
+  </si>
+  <si>
+    <t>Stakeholder: Markus. Indirekte Nutzer: Entscheidungsgremium. Weitere Stakeholder: Studenten, Schulleitung, Institute.
+Hervorgehobene Stakeholder: Studenten.
+Initiale Stakeholderanalyse, damit der Prototyp sinnvoll umgesetzt werden kann.</t>
+  </si>
+  <si>
+    <t>Kreativfrage: Was ist die Konkurrenz? Aktuelles Whiteboard? Das Web?
+Konkurrenzanalyse: Kein anderer Anbieter, zumindest nicht “ab Stange”.
+Anwendung ist so neu, dass es einen Prototypen dafür braucht.</t>
+  </si>
+  <si>
+    <t>Müsste heissen: “Alle aus Szenarios ableitbare Features dokumentiert”.</t>
   </si>
 </sst>
 </file>
@@ -1219,71 +1235,71 @@
     </xf>
   </cellXfs>
   <cellStyles count="131">
-    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1349,42 +1365,11 @@
     <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="121">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1399,524 +1384,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1947,6 +1415,670 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1978,37 +2110,6 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2060,62 +2161,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -2147,36 +2193,6 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3378,34 +3394,48 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F34" totalsRowCount="1" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48">
   <autoFilter ref="A4:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="6" name="G" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="3" name="N" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="5" name="besprochen am" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="1" name="#" dataDxfId="47" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="46" totalsRowDxfId="4"/>
+    <tableColumn id="6" name="G" dataDxfId="45" totalsRowDxfId="3"/>
+    <tableColumn id="3" name="N" dataDxfId="44" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="43" totalsRowDxfId="1"/>
+    <tableColumn id="5" name="besprochen am" dataDxfId="42" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:E93" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:E93" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
   <autoFilter ref="A87:E93"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="32"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="31"/>
-    <tableColumn id="5" name="G" dataDxfId="30"/>
-    <tableColumn id="3" name="N" dataDxfId="29"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="28"/>
+    <tableColumn id="1" name="#" dataDxfId="38"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="37"/>
+    <tableColumn id="5" name="G" dataDxfId="36"/>
+    <tableColumn id="3" name="N" dataDxfId="35"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:E83" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:E83" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
   <autoFilter ref="A78:E83"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="#" dataDxfId="30"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="29"/>
+    <tableColumn id="5" name="G" dataDxfId="28"/>
+    <tableColumn id="3" name="N" dataDxfId="27"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="26"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E145" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A138:E145"/>
   <tableColumns count="5">
     <tableColumn id="1" name="#" dataDxfId="24"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="23"/>
@@ -3417,9 +3447,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E145" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A138:E145"/>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A125:E135"/>
   <tableColumns count="5">
     <tableColumn id="1" name="#" dataDxfId="18"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="17"/>
@@ -3431,29 +3461,15 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="13">
-  <autoFilter ref="A125:E135"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="12"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="11"/>
-    <tableColumn id="5" name="G" dataDxfId="10"/>
-    <tableColumn id="3" name="N" dataDxfId="9"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="8"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table152" displayName="Table152" ref="A173:E176" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table152" displayName="Table152" ref="A173:E176" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="A173:E176"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="4"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="3"/>
-    <tableColumn id="5" name="G" dataDxfId="2"/>
-    <tableColumn id="3" name="N" dataDxfId="1"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="10"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="9"/>
+    <tableColumn id="5" name="G" dataDxfId="8"/>
+    <tableColumn id="3" name="N" dataDxfId="7"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3572,9 +3588,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3612,7 +3628,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -3684,7 +3700,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3863,11 +3879,11 @@
   </sheetPr>
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F196" sqref="F196"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="120.85546875" customWidth="1"/>
@@ -4076,7 +4092,9 @@
       </c>
       <c r="D14"/>
       <c r="E14"/>
-      <c r="F14" s="71"/>
+      <c r="F14" s="71" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A15" s="9">
@@ -4964,7 +4982,7 @@
       <c r="D80" s="33"/>
       <c r="E80" s="38"/>
     </row>
-    <row r="81" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>3</v>
       </c>
@@ -4975,9 +4993,11 @@
         <v>5</v>
       </c>
       <c r="D81" s="33"/>
-      <c r="E81" s="38"/>
-    </row>
-    <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E81" s="38" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="9">
         <v>4</v>
       </c>
@@ -4988,7 +5008,9 @@
         <v>5</v>
       </c>
       <c r="D82" s="33"/>
-      <c r="E82" s="38"/>
+      <c r="E82" s="38" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
@@ -5215,7 +5237,7 @@
       <c r="D100" s="33"/>
       <c r="E100" s="38"/>
     </row>
-    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="9">
         <v>5</v>
       </c>
@@ -5226,7 +5248,9 @@
         <v>0</v>
       </c>
       <c r="D101" s="33"/>
-      <c r="E101" s="38"/>
+      <c r="E101" s="38" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
@@ -6610,7 +6634,7 @@
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -6630,7 +6654,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
refs #842 übrige Kriterien übernommen
Former-commit-id: 413269984e093e8cd4f3e4a685e501b6c8620bfc
</commit_message>
<xml_diff>
--- a/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
+++ b/doc/vorgaben/Kriterien SA-BA Stolze 2012 FS.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="192">
   <si>
     <t>#</t>
   </si>
@@ -536,9 +536,6 @@
   </si>
   <si>
     <t>Tests durch Screenshots dokumentieren</t>
-  </si>
-  <si>
-    <t>Installationsanleitung nur sofern HW bis dann vorhanden</t>
   </si>
   <si>
     <t>W</t>
@@ -653,6 +650,22 @@
   </si>
   <si>
     <t>Müsste heissen: “Alle aus Szenarios ableitbare Features dokumentiert”.</t>
+  </si>
+  <si>
+    <t>Zu Postern: von wo kommen sie (Sekretariat)</t>
+  </si>
+  <si>
+    <t>Es sind Elemente in der Lösung, wo finde ich die im Domain Modell</t>
+  </si>
+  <si>
+    <t>Umfrage: viele Studenten befragt. 
+Andere Dinge mit wenig Personen durchgeführt: Resultate waren so deutlich, dass die statistische Analyse nicht notwendig war. Wenn es Tests gibt, die nicht gemacht wurden plausibel begründen.</t>
+  </si>
+  <si>
+    <t>Hardwareconfig &amp; Softwareconfig dokumentieren</t>
+  </si>
+  <si>
+    <t>14.5.2012: Auf 0 setzen</t>
   </si>
 </sst>
 </file>
@@ -1028,7 +1041,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1233,6 +1246,7 @@
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="131">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1370,6 +1384,37 @@
   <dxfs count="121">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1384,7 +1429,524 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Calibri"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1415,670 +1977,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF505050"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Calibri"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2110,6 +2008,37 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF505050"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2161,7 +2090,62 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2193,6 +2177,36 @@
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241921"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -3394,48 +3408,34 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:F34" totalsRowCount="1" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48">
   <autoFilter ref="A4:F33"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="#" dataDxfId="47" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="46" totalsRowDxfId="4"/>
-    <tableColumn id="6" name="G" dataDxfId="45" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="N" dataDxfId="44" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="43" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="besprochen am" dataDxfId="42" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="#" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="6" name="G" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="3" name="N" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="5" name="besprochen am" dataDxfId="37" totalsRowDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:E93" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table715" displayName="Table715" ref="A87:E93" totalsRowShown="0" headerRowDxfId="35" headerRowBorderDxfId="34" tableBorderDxfId="33">
   <autoFilter ref="A87:E93"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="38"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="37"/>
-    <tableColumn id="5" name="G" dataDxfId="36"/>
-    <tableColumn id="3" name="N" dataDxfId="35"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="34"/>
+    <tableColumn id="1" name="#" dataDxfId="32"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="31"/>
+    <tableColumn id="5" name="G" dataDxfId="30"/>
+    <tableColumn id="3" name="N" dataDxfId="29"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:E83" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table71518" displayName="Table71518" ref="A78:E83" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25">
   <autoFilter ref="A78:E83"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="30"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="29"/>
-    <tableColumn id="5" name="G" dataDxfId="28"/>
-    <tableColumn id="3" name="N" dataDxfId="27"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="26"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E145" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A138:E145"/>
   <tableColumns count="5">
     <tableColumn id="1" name="#" dataDxfId="24"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="23"/>
@@ -3447,9 +3447,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="19">
-  <autoFilter ref="A125:E135"/>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table1020" displayName="Table1020" ref="A138:E145" totalsRowShown="0" headerRowDxfId="19">
+  <autoFilter ref="A138:E145"/>
   <tableColumns count="5">
     <tableColumn id="1" name="#" dataDxfId="18"/>
     <tableColumn id="2" name="Beschreibung" dataDxfId="17"/>
@@ -3461,15 +3461,29 @@
 </table>
 </file>
 
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table1021" displayName="Table1021" ref="A125:E135" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="A125:E135"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="#" dataDxfId="12"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="11"/>
+    <tableColumn id="5" name="G" dataDxfId="10"/>
+    <tableColumn id="3" name="N" dataDxfId="9"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table152" displayName="Table152" ref="A173:E176" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table152" displayName="Table152" ref="A173:E176" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A173:E176"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="#" dataDxfId="10"/>
-    <tableColumn id="2" name="Beschreibung" dataDxfId="9"/>
-    <tableColumn id="5" name="G" dataDxfId="8"/>
-    <tableColumn id="3" name="N" dataDxfId="7"/>
-    <tableColumn id="4" name="Kommentar" dataDxfId="6"/>
+    <tableColumn id="1" name="#" dataDxfId="4"/>
+    <tableColumn id="2" name="Beschreibung" dataDxfId="3"/>
+    <tableColumn id="5" name="G" dataDxfId="2"/>
+    <tableColumn id="3" name="N" dataDxfId="1"/>
+    <tableColumn id="4" name="Kommentar" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3879,8 +3893,8 @@
   </sheetPr>
   <dimension ref="A1:F207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E176" sqref="E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3997,7 +4011,7 @@
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8" s="72" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -4005,7 +4019,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C9" s="40">
         <v>5</v>
@@ -4013,7 +4027,7 @@
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9" s="71" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -4077,7 +4091,7 @@
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13" s="71" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -4093,7 +4107,7 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14" s="71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -4109,7 +4123,7 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15" s="71" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
@@ -4217,7 +4231,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="40">
         <v>5</v>
@@ -4286,7 +4300,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C28" s="40">
         <v>5</v>
@@ -4300,7 +4314,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C29" s="40">
         <v>5</v>
@@ -4342,7 +4356,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="40">
         <v>5</v>
@@ -4426,7 +4440,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38" s="32">
         <v>5</v>
@@ -4508,7 +4522,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C44" s="32">
         <v>5</v>
@@ -4994,7 +5008,7 @@
       </c>
       <c r="D81" s="33"/>
       <c r="E81" s="38" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -5009,7 +5023,7 @@
       </c>
       <c r="D82" s="33"/>
       <c r="E82" s="38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5024,7 +5038,7 @@
       </c>
       <c r="D83" s="33"/>
       <c r="E83" s="38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="85" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5216,7 +5230,7 @@
         <v>3</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C99" s="34">
         <v>5</v>
@@ -5229,7 +5243,7 @@
         <v>4</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C100" s="34">
         <v>5</v>
@@ -5249,7 +5263,7 @@
       </c>
       <c r="D101" s="33"/>
       <c r="E101" s="38" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5364,15 +5378,17 @@
         <v>3</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C110" s="34">
         <v>5</v>
       </c>
       <c r="D110" s="33"/>
-      <c r="E110" s="38"/>
-    </row>
-    <row r="111" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E110" s="38" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="5">
         <v>4</v>
       </c>
@@ -5383,7 +5399,9 @@
         <v>5</v>
       </c>
       <c r="D111" s="33"/>
-      <c r="E111" s="38"/>
+      <c r="E111" s="38" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="112" spans="1:6" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B112" s="54"/>
@@ -5443,7 +5461,7 @@
         <v>2</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C116" s="34">
         <v>5</v>
@@ -5521,14 +5539,14 @@
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C122" s="34">
         <v>0</v>
       </c>
       <c r="D122" s="33"/>
       <c r="E122" s="38" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="123" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5635,7 +5653,7 @@
       </c>
       <c r="D130" s="33"/>
       <c r="E130" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -5643,7 +5661,7 @@
         <v>6</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C131" s="34">
         <v>5</v>
@@ -5669,7 +5687,7 @@
         <v>8</v>
       </c>
       <c r="B133" s="54" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C133" s="34">
         <v>5</v>
@@ -5695,7 +5713,7 @@
         <v>10</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C135" s="34">
         <v>5</v>
@@ -5795,7 +5813,7 @@
       <c r="D142" s="33"/>
       <c r="E142" s="38"/>
     </row>
-    <row r="143" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A143" s="5">
         <v>6</v>
       </c>
@@ -5806,7 +5824,9 @@
         <v>3</v>
       </c>
       <c r="D143" s="33"/>
-      <c r="E143" s="38"/>
+      <c r="E143" s="38" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="144" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
@@ -5971,7 +5991,7 @@
       </c>
       <c r="D156" s="33"/>
       <c r="E156" s="38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5986,7 +6006,7 @@
       </c>
       <c r="D157" s="33"/>
       <c r="E157" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -6116,8 +6136,8 @@
         <v>5</v>
       </c>
       <c r="D167" s="33"/>
-      <c r="E167" s="38" t="s">
-        <v>151</v>
+      <c r="E167" s="80" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="168" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -6166,10 +6186,10 @@
     </row>
     <row r="172" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A172" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="B172" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="B172" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="C172" s="7"/>
       <c r="D172" s="28" t="s">
@@ -6202,7 +6222,7 @@
         <v>1</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C174" s="34">
         <v>5</v>
@@ -6215,20 +6235,22 @@
         <v>2</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C175" s="34">
         <v>0</v>
       </c>
       <c r="D175" s="33"/>
-      <c r="E175" s="38"/>
+      <c r="E175" s="38" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="176" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="5">
         <v>3</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C176" s="34">
         <v>5</v>
@@ -6242,7 +6264,7 @@
       </c>
       <c r="E178" s="67"/>
       <c r="F178" s="73" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="179" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
@@ -6533,10 +6555,10 @@
     </row>
     <row r="196" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A196" s="48" t="s">
+        <v>160</v>
+      </c>
+      <c r="B196" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="B196" s="10" t="s">
-        <v>162</v>
       </c>
       <c r="C196" s="50"/>
       <c r="D196" s="49" t="s">
@@ -6573,7 +6595,7 @@
     </row>
     <row r="200" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B200" s="47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E200" s="76">
         <f>((E179*F179)+E184*F184+E197*F197)/(F179+F184+F197)</f>
@@ -6658,12 +6680,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>